<commit_message>
Updated translation by Ioannis
</commit_message>
<xml_diff>
--- a/material/translation/PersonGenderEnum.xlsx
+++ b/material/translation/PersonGenderEnum.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ihuedu.sharepoint.com/sites/--/Shared Documents/DE4A/WP3/XSDs/Ana Rosa/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="7" documentId="11_2788439F66335EC9CE631B9311B594C83ADE0C1D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AB281FF2-7591-4B22-9253-F5681566DFE9}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="7755"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="fr" sheetId="6" r:id="rId1"/>
@@ -14,12 +20,23 @@
     <sheet name="en" sheetId="2" r:id="rId5"/>
     <sheet name="Terms" sheetId="4" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="19">
   <si>
     <t>Term</t>
   </si>
@@ -66,17 +83,34 @@
     <t>PersonGenderEnum/Female</t>
   </si>
   <si>
-    <t>PersonGenderEnum/Other</t>
+    <t>PersonGenderEnum/NAP</t>
+  </si>
+  <si>
+    <t>PersonGenderEnum/NKN</t>
+  </si>
+  <si>
+    <t>PersonGenderEnum/NST</t>
+  </si>
+  <si>
+    <t>Human Sex</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -99,15 +133,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -116,12 +153,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -163,7 +203,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -196,9 +236,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -231,6 +288,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -406,19 +480,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -435,7 +509,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="str">
         <f>Terms!A2</f>
         <v>PersonGenderEnum</v>
@@ -444,52 +518,52 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="str">
         <f>Terms!A3</f>
-        <v>PersonGenderEnum/Male</v>
+        <v>PersonGenderEnum/Female</v>
       </c>
       <c r="E3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="str">
         <f>Terms!A4</f>
-        <v>PersonGenderEnum/Female</v>
+        <v>PersonGenderEnum/Male</v>
       </c>
       <c r="E4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="str">
         <f>Terms!A5</f>
-        <v>PersonGenderEnum/Other</v>
+        <v>PersonGenderEnum/NAP</v>
       </c>
       <c r="E5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="str">
         <f>Terms!A6</f>
-        <v>0</v>
+        <v>PersonGenderEnum/NKN</v>
       </c>
       <c r="E6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="str">
         <f>Terms!A7</f>
-        <v>0</v>
+        <v>PersonGenderEnum/NST</v>
       </c>
       <c r="E7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <f>Terms!A8</f>
         <v>0</v>
@@ -498,7 +572,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
         <f>Terms!A9</f>
         <v>0</v>
@@ -507,7 +581,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
         <f>Terms!A10</f>
         <v>0</v>
@@ -517,7 +591,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
         <f>Terms!A11</f>
         <v>0</v>
@@ -526,13 +600,13 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
         <f>Terms!A12</f>
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
         <f>Terms!A13</f>
         <v>0</v>
@@ -544,19 +618,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -573,7 +647,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="str">
         <f>Terms!A2</f>
         <v>PersonGenderEnum</v>
@@ -582,52 +656,52 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="str">
         <f>Terms!A3</f>
-        <v>PersonGenderEnum/Male</v>
+        <v>PersonGenderEnum/Female</v>
       </c>
       <c r="E3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="str">
         <f>Terms!A4</f>
-        <v>PersonGenderEnum/Female</v>
+        <v>PersonGenderEnum/Male</v>
       </c>
       <c r="E4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="str">
         <f>Terms!A5</f>
-        <v>PersonGenderEnum/Other</v>
+        <v>PersonGenderEnum/NAP</v>
       </c>
       <c r="E5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="str">
         <f>Terms!A6</f>
-        <v>0</v>
+        <v>PersonGenderEnum/NKN</v>
       </c>
       <c r="E6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="str">
         <f>Terms!A7</f>
-        <v>0</v>
+        <v>PersonGenderEnum/NST</v>
       </c>
       <c r="E7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <f>Terms!A8</f>
         <v>0</v>
@@ -636,7 +710,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
         <f>Terms!A9</f>
         <v>0</v>
@@ -645,7 +719,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
         <f>Terms!A10</f>
         <v>0</v>
@@ -655,7 +729,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
         <f>Terms!A11</f>
         <v>0</v>
@@ -664,13 +738,13 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
         <f>Terms!A12</f>
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
         <f>Terms!A13</f>
         <v>0</v>
@@ -682,19 +756,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -711,7 +785,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="str">
         <f>Terms!A2</f>
         <v>PersonGenderEnum</v>
@@ -720,52 +794,52 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="str">
         <f>Terms!A3</f>
-        <v>PersonGenderEnum/Male</v>
+        <v>PersonGenderEnum/Female</v>
       </c>
       <c r="E3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="str">
         <f>Terms!A4</f>
-        <v>PersonGenderEnum/Female</v>
+        <v>PersonGenderEnum/Male</v>
       </c>
       <c r="E4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="str">
         <f>Terms!A5</f>
-        <v>PersonGenderEnum/Other</v>
+        <v>PersonGenderEnum/NAP</v>
       </c>
       <c r="E5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="str">
         <f>Terms!A6</f>
-        <v>0</v>
+        <v>PersonGenderEnum/NKN</v>
       </c>
       <c r="E6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="str">
         <f>Terms!A7</f>
-        <v>0</v>
+        <v>PersonGenderEnum/NST</v>
       </c>
       <c r="E7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <f>Terms!A8</f>
         <v>0</v>
@@ -774,7 +848,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
         <f>Terms!A9</f>
         <v>0</v>
@@ -783,7 +857,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
         <f>Terms!A10</f>
         <v>0</v>
@@ -793,7 +867,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
         <f>Terms!A11</f>
         <v>0</v>
@@ -802,13 +876,13 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
         <f>Terms!A12</f>
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
         <f>Terms!A13</f>
         <v>0</v>
@@ -820,22 +894,22 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="36" customWidth="1"/>
-    <col min="2" max="2" width="24.5703125" customWidth="1"/>
+    <col min="2" max="2" width="24.5546875" customWidth="1"/>
     <col min="3" max="3" width="79" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -852,7 +926,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="str">
         <f>Terms!A2</f>
         <v>PersonGenderEnum</v>
@@ -861,52 +935,52 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="str">
         <f>Terms!A3</f>
-        <v>PersonGenderEnum/Male</v>
+        <v>PersonGenderEnum/Female</v>
       </c>
       <c r="E3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="str">
         <f>Terms!A4</f>
-        <v>PersonGenderEnum/Female</v>
+        <v>PersonGenderEnum/Male</v>
       </c>
       <c r="E4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="str">
         <f>Terms!A5</f>
-        <v>PersonGenderEnum/Other</v>
+        <v>PersonGenderEnum/NAP</v>
       </c>
       <c r="E5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="str">
         <f>Terms!A6</f>
-        <v>0</v>
+        <v>PersonGenderEnum/NKN</v>
       </c>
       <c r="E6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="str">
         <f>Terms!A7</f>
-        <v>0</v>
+        <v>PersonGenderEnum/NST</v>
       </c>
       <c r="E7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <f>Terms!A8</f>
         <v>0</v>
@@ -915,7 +989,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
         <f>Terms!A9</f>
         <v>0</v>
@@ -924,7 +998,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
         <f>Terms!A10</f>
         <v>0</v>
@@ -934,7 +1008,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
         <f>Terms!A11</f>
         <v>0</v>
@@ -943,43 +1017,43 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
         <f>Terms!A12</f>
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
         <f>Terms!A13</f>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14">
         <f>Terms!A14</f>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15">
         <f>Terms!A15</f>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16">
         <f>Terms!A16</f>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17">
         <f>Terms!A15</f>
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18">
         <f>Terms!A16</f>
         <v>0</v>
@@ -991,21 +1065,21 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2:D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="65.42578125" customWidth="1"/>
+    <col min="1" max="1" width="25.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="65.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1022,7 +1096,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="str">
         <f>Terms!A2</f>
         <v>PersonGenderEnum</v>
@@ -1031,52 +1105,52 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="str">
         <f>Terms!A3</f>
-        <v>PersonGenderEnum/Male</v>
+        <v>PersonGenderEnum/Female</v>
       </c>
       <c r="E3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="str">
         <f>Terms!A4</f>
-        <v>PersonGenderEnum/Female</v>
+        <v>PersonGenderEnum/Male</v>
       </c>
       <c r="E4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="str">
         <f>Terms!A5</f>
-        <v>PersonGenderEnum/Other</v>
+        <v>PersonGenderEnum/NAP</v>
       </c>
       <c r="E5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="str">
         <f>Terms!A6</f>
-        <v>0</v>
+        <v>PersonGenderEnum/NKN</v>
       </c>
       <c r="E6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="str">
         <f>Terms!A7</f>
-        <v>0</v>
+        <v>PersonGenderEnum/NST</v>
       </c>
       <c r="E7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <f>Terms!A8</f>
         <v>0</v>
@@ -1085,7 +1159,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
         <f>Terms!A9</f>
         <v>0</v>
@@ -1094,7 +1168,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
         <f>Terms!A10</f>
         <v>0</v>
@@ -1104,7 +1178,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
         <f>Terms!A11</f>
         <v>0</v>
@@ -1113,43 +1187,43 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
         <f>Terms!A12</f>
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
         <f>Terms!A13</f>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14">
         <f>Terms!A14</f>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15">
         <f>Terms!A15</f>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16">
         <f>Terms!A14</f>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17">
         <f>Terms!A15</f>
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18">
         <f>Terms!A16</f>
         <v>0</v>
@@ -1161,20 +1235,20 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.140625" customWidth="1"/>
+    <col min="1" max="1" width="32.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -1188,39 +1262,314 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>12</v>
       </c>
+      <c r="B2" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="C2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>18</v>
       </c>
       <c r="C3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>13</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>18</v>
       </c>
       <c r="C4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>15</v>
       </c>
+      <c r="B5" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="C5" t="s">
         <v>11</v>
       </c>
     </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2:B7" r:id="rId1" display="https://op.europa.eu/en/web/eu-vocabularies/at-concept-scheme/-/resource/authority/human-sex/?target=Browse&amp;uri=http://publications.europa.eu/resource/authority/human-sex" xr:uid="{DFF505D8-07A4-43C6-B722-03F97B3CA091}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Έγγραφο" ma:contentTypeID="0x0101007E289342E878A3439E8711FFF848F32F" ma:contentTypeVersion="11" ma:contentTypeDescription="Δημιουργία νέου εγγράφου" ma:contentTypeScope="" ma:versionID="46ceb6b1ca17f648485ffad8d87a7461">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="387b4333-7bd0-482a-b673-9a586eb2ceee" xmlns:ns3="4aa09831-7f3d-42ba-9b8c-49994d1626d2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a21b98261e948a646c8dae0c6b0aefd5" ns2:_="" ns3:_="">
+    <xsd:import namespace="387b4333-7bd0-482a-b673-9a586eb2ceee"/>
+    <xsd:import namespace="4aa09831-7f3d-42ba-9b8c-49994d1626d2"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoTags" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="387b4333-7bd0-482a-b673-9a586eb2ceee" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="10" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceKeyPoints" ma:index="11" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="12" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoTags" ma:index="13" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="14" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="15" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="16" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="4aa09831-7f3d-42ba-9b8c-49994d1626d2" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="SharedWithUsers" ma:index="17" nillable="true" ma:displayName="Κοινή χρήση με" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="18" nillable="true" ma:displayName="Κοινή χρήση με λεπτομέρειες" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Τύπος περιεχομένου"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Τίτλος"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2A0DCFF2-9E5C-48A3-B79F-386263CF1D34}"/>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{34E986EC-7FDC-43C1-9D89-AA0303DD8FF9}"/>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{92927983-0A51-4957-B167-416398CE4BA2}"/>
 </file>
</xml_diff>